<commit_message>
seperated strata_fee from row_data
</commit_message>
<xml_diff>
--- a/raw_data_100087848963_2023-07-21.xlsx
+++ b/raw_data_100087848963_2023-07-21.xlsx
@@ -8,24 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\DataAnalystCertificate\projects\ShodaClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92A7817-CCFD-4D5D-A9DF-2D1A4A76B33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43206B60-629D-4509-99D9-E11DD44A838E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
     <sheet name="clean_data" sheetId="2" r:id="rId2"/>
-    <sheet name="strata_fee" sheetId="4" r:id="rId3"/>
-    <sheet name="sf_pivot" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">clean_data!$A$1:$G$75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw_data!$C$1:$C$221</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId5"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -364,222 +359,6 @@
   </si>
   <si>
     <t>DONGLI LIU</t>
-  </si>
-  <si>
-    <t>Payer</t>
-  </si>
-  <si>
-    <t>Ref</t>
-  </si>
-  <si>
-    <t>20230705194805814315</t>
-  </si>
-  <si>
-    <t>20230704154714813333</t>
-  </si>
-  <si>
-    <t>20230701204439814025</t>
-  </si>
-  <si>
-    <t>20230630054126813522</t>
-  </si>
-  <si>
-    <t>20230606083305814404</t>
-  </si>
-  <si>
-    <t>20230530163859814369</t>
-  </si>
-  <si>
-    <t>20230501180206814051</t>
-  </si>
-  <si>
-    <t>20230501145741813217</t>
-  </si>
-  <si>
-    <t>20230501134933813315</t>
-  </si>
-  <si>
-    <t>20230501121028813801</t>
-  </si>
-  <si>
-    <t>20230501120957814861</t>
-  </si>
-  <si>
-    <t>20230501120924814853</t>
-  </si>
-  <si>
-    <t>20230428193105814655</t>
-  </si>
-  <si>
-    <t>20230401134832814898</t>
-  </si>
-  <si>
-    <t>20230331072337813777</t>
-  </si>
-  <si>
-    <t>20230331054355813952</t>
-  </si>
-  <si>
-    <t>20230330142222812860</t>
-  </si>
-  <si>
-    <t>20230302153502814406</t>
-  </si>
-  <si>
-    <t>20230302072719812526</t>
-  </si>
-  <si>
-    <t>20230302072641814718</t>
-  </si>
-  <si>
-    <t>20230301190435812268</t>
-  </si>
-  <si>
-    <t>20230228221740814067</t>
-  </si>
-  <si>
-    <t>20230224112033813292</t>
-  </si>
-  <si>
-    <t>20230201161250812564</t>
-  </si>
-  <si>
-    <t>20230201065125813526</t>
-  </si>
-  <si>
-    <t>20230131215635814230</t>
-  </si>
-  <si>
-    <t>20230131110332814029</t>
-  </si>
-  <si>
-    <t>20230102094259813200</t>
-  </si>
-  <si>
-    <t>20230101140733813853</t>
-  </si>
-  <si>
-    <t>20221231070111814838</t>
-  </si>
-  <si>
-    <t>20221226233450814041</t>
-  </si>
-  <si>
-    <t>20221226233254813811</t>
-  </si>
-  <si>
-    <t>20221205091159812301</t>
-  </si>
-  <si>
-    <t>20221205052515813993</t>
-  </si>
-  <si>
-    <t>20221201102153812851</t>
-  </si>
-  <si>
-    <t>20221201074144812391</t>
-  </si>
-  <si>
-    <t>20221113211305814568</t>
-  </si>
-  <si>
-    <t>20221101105446812447</t>
-  </si>
-  <si>
-    <t>20221101092556413389</t>
-  </si>
-  <si>
-    <t>20221101082525413535</t>
-  </si>
-  <si>
-    <t>20221028203342413005</t>
-  </si>
-  <si>
-    <t>20221003232656203286</t>
-  </si>
-  <si>
-    <t>20221002100802201926</t>
-  </si>
-  <si>
-    <t>20221002053814203736</t>
-  </si>
-  <si>
-    <t>20220930165853202439</t>
-  </si>
-  <si>
-    <t>20220929043741201423</t>
-  </si>
-  <si>
-    <t>20220908233924202662</t>
-  </si>
-  <si>
-    <t>20220901151903203839</t>
-  </si>
-  <si>
-    <t>20220831214519202877</t>
-  </si>
-  <si>
-    <t>20220831164741203790</t>
-  </si>
-  <si>
-    <t>20220801153101201465</t>
-  </si>
-  <si>
-    <t>20220801103412201168</t>
-  </si>
-  <si>
-    <t>20220731110626668921</t>
-  </si>
-  <si>
-    <t>20220730090736203088</t>
-  </si>
-  <si>
-    <t>20220729074647203140</t>
-  </si>
-  <si>
-    <t>20220701112019203867</t>
-  </si>
-  <si>
-    <t>20220701081603201499</t>
-  </si>
-  <si>
-    <t>20220629224708202856</t>
-  </si>
-  <si>
-    <t>20220629162419203595</t>
-  </si>
-  <si>
-    <t>20220629150729201494</t>
-  </si>
-  <si>
-    <t>20220603154529666891</t>
-  </si>
-  <si>
-    <t>20220603095407666866</t>
-  </si>
-  <si>
-    <t>20220602084104666385</t>
-  </si>
-  <si>
-    <t>20220531130341666708</t>
-  </si>
-  <si>
-    <t>20220527095424662054</t>
-  </si>
-  <si>
-    <t>Pay Method</t>
-  </si>
-  <si>
-    <t>Sum of Amount</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>EDWINALBERT IMHOFF</t>
   </si>
 </sst>
 </file>
@@ -732,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -783,7 +562,7 @@
     <xf numFmtId="15" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -792,32 +571,26 @@
     <xf numFmtId="15" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="8" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,574 +607,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dongli" refreshedDate="45128.478500231482" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="65" xr:uid="{E93254BA-6910-4E43-8DBD-AF066E9BDCAC}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E66" sheet="strata_fee"/>
-  </cacheSource>
-  <cacheFields count="5">
-    <cacheField name="Date" numFmtId="15">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2022-05-27T00:00:00" maxDate="2023-07-06T00:00:00"/>
-    </cacheField>
-    <cacheField name="Amount" numFmtId="8">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="150" maxValue="600"/>
-    </cacheField>
-    <cacheField name="Pay Method" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Ref" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Payer" numFmtId="0">
-      <sharedItems count="11">
-        <s v="DONGLI LIU"/>
-        <s v="EDWINALBERT IMHOFF"/>
-        <s v="XIAOPENG FENG"/>
-        <s v="TRACY CARRIER"/>
-        <s v="SIDDHARTH SINHA"/>
-        <s v="DONGLILIU" u="1"/>
-        <s v="XIAOPENGFENG" u="1"/>
-        <s v="TRACYCARRIER" u="1"/>
-        <s v="EDWINALBERTIMHOFF" u="1"/>
-        <s v="SIDDHARTHSINHA" u="1"/>
-        <s v="EDWIN ALBERT IMHOFF" u="1"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="65">
-  <r>
-    <d v="2023-07-05T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230705194805814315"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2023-07-04T00:00:00"/>
-    <n v="300"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230704154714813333"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2023-07-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230701204439814025"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2023-06-30T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230630054126813522"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2023-06-06T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230606083305814404"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2023-05-30T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230530163859814369"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2023-05-01T00:00:00"/>
-    <n v="300"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230501180206814051"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2023-05-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230501145741813217"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2023-05-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230501134933813315"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2023-05-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230501121028813801"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2023-05-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230501120957814861"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2023-05-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230501120924814853"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2023-04-28T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230428193105814655"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2023-04-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230401134832814898"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2023-03-31T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230331072337813777"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2023-03-31T00:00:00"/>
-    <n v="300"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230331054355813952"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2023-03-30T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230330142222812860"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2023-03-02T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230302153502814406"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2023-03-02T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230302072719812526"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2023-03-02T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230302072641814718"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2023-03-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230301190435812268"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2023-03-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230228221740814067"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2023-02-24T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230224112033813292"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2023-02-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230201161250812564"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2023-02-01T00:00:00"/>
-    <n v="300"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230201065125813526"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2023-02-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230131215635814230"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2023-01-31T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230131110332814029"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2023-01-02T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230102094259813200"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2023-01-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20230101140733813853"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2022-12-31T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221231070111814838"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2022-12-27T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221226233450814041"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2022-12-27T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221226233254813811"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2022-12-05T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221205091159812301"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2022-12-05T00:00:00"/>
-    <n v="300"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221205052515813993"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2022-12-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221201102153812851"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2022-12-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221201074144812391"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2022-11-14T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221113211305814568"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2022-11-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221101105446812447"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2022-11-01T00:00:00"/>
-    <n v="300"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221101092556413389"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2022-11-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221101082525413535"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2022-10-28T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221028203342413005"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2022-10-04T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221003232656203286"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2022-10-02T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221002100802201926"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2022-10-02T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20221002053814203736"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2022-09-30T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220930165853202439"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2022-09-29T00:00:00"/>
-    <n v="600"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220929043741201423"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2022-09-09T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220908233924202662"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2022-09-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220901151903203839"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2022-09-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220831214519202877"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2022-08-31T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220831164741203790"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2022-08-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220801153101201465"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2022-08-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220801103412201168"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2022-07-31T00:00:00"/>
-    <n v="300"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220731110626668921"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2022-07-30T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220730090736203088"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2022-07-29T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220729074647203140"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2022-07-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220701112019203867"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2022-07-01T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220701081603201499"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2022-06-30T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220629224708202856"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2022-06-29T00:00:00"/>
-    <n v="300"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220629162419203595"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2022-06-29T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220629150729201494"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2022-06-03T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220603154529666891"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <d v="2022-06-03T00:00:00"/>
-    <n v="300"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220603095407666866"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2022-06-02T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220602084104666385"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2022-05-31T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220531130341666708"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2022-05-27T00:00:00"/>
-    <n v="150"/>
-    <s v="e-Transfer credit"/>
-    <s v="20220527095424662054"/>
-    <x v="0"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF19025F-1016-4A7A-A2B4-7153ABDA26AA}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField numFmtId="15" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item m="1" x="10"/>
-        <item m="1" x="8"/>
-        <item x="4"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item m="1" x="6"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Amount" fld="1" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1705,7 +910,7 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="26">
         <v>-2310</v>
       </c>
       <c r="D2" s="19">
@@ -1717,7 +922,7 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4">
@@ -1725,7 +930,7 @@
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:4" ht="20.399999999999999" customHeight="1">
@@ -1733,7 +938,7 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:4" ht="20.399999999999999">
@@ -1743,10 +948,10 @@
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="21">
-        <v>150</v>
-      </c>
-      <c r="D6" s="22">
+      <c r="C6" s="27">
+        <v>150</v>
+      </c>
+      <c r="D6" s="24">
         <v>10015</v>
       </c>
     </row>
@@ -1755,16 +960,16 @@
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999">
       <c r="A8" s="20"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:4" ht="20.399999999999999">
       <c r="A9" s="17">
@@ -1773,7 +978,7 @@
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="18">
         <v>300</v>
       </c>
       <c r="D9" s="19">
@@ -1785,7 +990,7 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="23"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4" ht="30.6">
@@ -1793,7 +998,7 @@
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="19"/>
     </row>
     <row r="12" spans="1:4" ht="20.399999999999999">
@@ -1803,10 +1008,10 @@
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="21">
-        <v>150</v>
-      </c>
-      <c r="D12" s="22">
+      <c r="C12" s="27">
+        <v>150</v>
+      </c>
+      <c r="D12" s="24">
         <v>9565</v>
       </c>
     </row>
@@ -1815,16 +1020,16 @@
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:4" ht="30.6">
       <c r="A14" s="20"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:4" ht="20.399999999999999">
       <c r="A15" s="17">
@@ -1833,7 +1038,7 @@
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="18">
         <v>150</v>
       </c>
       <c r="D15" s="19">
@@ -1845,7 +1050,7 @@
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="19"/>
     </row>
     <row r="17" spans="1:4" ht="30.6">
@@ -1853,7 +1058,7 @@
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="19"/>
     </row>
     <row r="18" spans="1:4" ht="20.399999999999999">
@@ -1863,10 +1068,10 @@
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="21">
-        <v>150</v>
-      </c>
-      <c r="D18" s="22">
+      <c r="C18" s="27">
+        <v>150</v>
+      </c>
+      <c r="D18" s="24">
         <v>9265</v>
       </c>
     </row>
@@ -1875,16 +1080,16 @@
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="24"/>
     </row>
     <row r="20" spans="1:4" ht="20.399999999999999">
       <c r="A20" s="20"/>
       <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="24"/>
     </row>
     <row r="21" spans="1:4" ht="20.399999999999999">
       <c r="A21" s="17">
@@ -1893,7 +1098,7 @@
       <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="18">
         <v>150</v>
       </c>
       <c r="D21" s="19">
@@ -1905,7 +1110,7 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="23"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="19"/>
     </row>
     <row r="23" spans="1:4" ht="30.6">
@@ -1913,7 +1118,7 @@
       <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="23"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="19"/>
     </row>
     <row r="24" spans="1:4" ht="20.399999999999999">
@@ -1923,10 +1128,10 @@
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="27">
         <v>300</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="24">
         <v>8965</v>
       </c>
     </row>
@@ -1935,16 +1140,16 @@
       <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="24"/>
     </row>
     <row r="26" spans="1:4" ht="30.6">
       <c r="A26" s="20"/>
       <c r="B26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="1:4" ht="20.399999999999999">
       <c r="A27" s="17">
@@ -1953,7 +1158,7 @@
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="18">
         <v>150</v>
       </c>
       <c r="D27" s="19">
@@ -1965,7 +1170,7 @@
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="23"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="19"/>
     </row>
     <row r="29" spans="1:4" ht="20.399999999999999">
@@ -1973,7 +1178,7 @@
       <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="23"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="19"/>
     </row>
     <row r="30" spans="1:4" ht="20.399999999999999">
@@ -1983,10 +1188,10 @@
       <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="21">
-        <v>150</v>
-      </c>
-      <c r="D30" s="22">
+      <c r="C30" s="27">
+        <v>150</v>
+      </c>
+      <c r="D30" s="24">
         <v>8515</v>
       </c>
     </row>
@@ -1995,16 +1200,16 @@
       <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="24"/>
     </row>
     <row r="32" spans="1:4" ht="30.6">
       <c r="A32" s="20"/>
       <c r="B32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="24"/>
     </row>
     <row r="33" spans="1:4" ht="20.399999999999999">
       <c r="A33" s="17">
@@ -2013,7 +1218,7 @@
       <c r="B33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="23">
+      <c r="C33" s="18">
         <v>150</v>
       </c>
       <c r="D33" s="19">
@@ -2025,7 +1230,7 @@
       <c r="B34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="23"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="19"/>
     </row>
     <row r="35" spans="1:4" ht="30.6">
@@ -2033,7 +1238,7 @@
       <c r="B35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="23"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="19"/>
     </row>
     <row r="36" spans="1:4" ht="20.399999999999999">
@@ -2043,10 +1248,10 @@
       <c r="B36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="21">
-        <v>150</v>
-      </c>
-      <c r="D36" s="22">
+      <c r="C36" s="27">
+        <v>150</v>
+      </c>
+      <c r="D36" s="24">
         <v>8215</v>
       </c>
     </row>
@@ -2055,16 +1260,16 @@
       <c r="B37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="22"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="24"/>
     </row>
     <row r="38" spans="1:4" ht="30.6">
       <c r="A38" s="20"/>
       <c r="B38" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="22"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="24"/>
     </row>
     <row r="39" spans="1:4" ht="20.399999999999999">
       <c r="A39" s="17">
@@ -2073,7 +1278,7 @@
       <c r="B39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C39" s="18">
         <v>150</v>
       </c>
       <c r="D39" s="19">
@@ -2085,7 +1290,7 @@
       <c r="B40" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="23"/>
+      <c r="C40" s="18"/>
       <c r="D40" s="19"/>
     </row>
     <row r="41" spans="1:4" ht="30.6">
@@ -2093,7 +1298,7 @@
       <c r="B41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="23"/>
+      <c r="C41" s="18"/>
       <c r="D41" s="19"/>
     </row>
     <row r="42" spans="1:4" ht="20.399999999999999">
@@ -2103,10 +1308,10 @@
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="21">
-        <v>150</v>
-      </c>
-      <c r="D42" s="22">
+      <c r="C42" s="27">
+        <v>150</v>
+      </c>
+      <c r="D42" s="24">
         <v>7915</v>
       </c>
     </row>
@@ -2115,16 +1320,16 @@
       <c r="B43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="22"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="24"/>
     </row>
     <row r="44" spans="1:4" ht="30.6">
       <c r="A44" s="20"/>
       <c r="B44" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="22"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="24"/>
     </row>
     <row r="45" spans="1:4" ht="20.399999999999999">
       <c r="A45" s="17">
@@ -2133,7 +1338,7 @@
       <c r="B45" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="23">
+      <c r="C45" s="18">
         <v>150</v>
       </c>
       <c r="D45" s="19">
@@ -2145,7 +1350,7 @@
       <c r="B46" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="23"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="19"/>
     </row>
     <row r="47" spans="1:4" ht="30.6">
@@ -2153,7 +1358,7 @@
       <c r="B47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C47" s="23"/>
+      <c r="C47" s="18"/>
       <c r="D47" s="19"/>
     </row>
     <row r="48" spans="1:4" ht="20.399999999999999">
@@ -2163,10 +1368,10 @@
       <c r="B48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="21">
-        <v>150</v>
-      </c>
-      <c r="D48" s="22">
+      <c r="C48" s="27">
+        <v>150</v>
+      </c>
+      <c r="D48" s="24">
         <v>7615</v>
       </c>
     </row>
@@ -2175,16 +1380,16 @@
       <c r="B49" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="22"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="24"/>
     </row>
     <row r="50" spans="1:4" ht="30.6">
       <c r="A50" s="20"/>
       <c r="B50" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="22"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="24"/>
     </row>
     <row r="51" spans="1:4" ht="20.399999999999999">
       <c r="A51" s="17">
@@ -2193,7 +1398,7 @@
       <c r="B51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="23">
+      <c r="C51" s="18">
         <v>300</v>
       </c>
       <c r="D51" s="19">
@@ -2205,7 +1410,7 @@
       <c r="B52" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="23"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="19"/>
     </row>
     <row r="53" spans="1:4" ht="30.6">
@@ -2213,7 +1418,7 @@
       <c r="B53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="23"/>
+      <c r="C53" s="18"/>
       <c r="D53" s="19"/>
     </row>
     <row r="54" spans="1:4" ht="20.399999999999999">
@@ -2223,10 +1428,10 @@
       <c r="B54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="21">
-        <v>150</v>
-      </c>
-      <c r="D54" s="22">
+      <c r="C54" s="27">
+        <v>150</v>
+      </c>
+      <c r="D54" s="24">
         <v>7165</v>
       </c>
     </row>
@@ -2235,16 +1440,16 @@
       <c r="B55" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="21"/>
-      <c r="D55" s="22"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="24"/>
     </row>
     <row r="56" spans="1:4" ht="20.399999999999999">
       <c r="A56" s="20"/>
       <c r="B56" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="21"/>
-      <c r="D56" s="22"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="24"/>
     </row>
     <row r="57" spans="1:4" ht="20.399999999999999">
       <c r="A57" s="17">
@@ -2253,7 +1458,7 @@
       <c r="B57" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="23">
+      <c r="C57" s="18">
         <v>150</v>
       </c>
       <c r="D57" s="19">
@@ -2265,7 +1470,7 @@
       <c r="B58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="23"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="19"/>
     </row>
     <row r="59" spans="1:4" ht="20.399999999999999">
@@ -2273,7 +1478,7 @@
       <c r="B59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="23"/>
+      <c r="C59" s="18"/>
       <c r="D59" s="19"/>
     </row>
     <row r="60" spans="1:4" ht="20.399999999999999">
@@ -2283,10 +1488,10 @@
       <c r="B60" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="21">
-        <v>150</v>
-      </c>
-      <c r="D60" s="22">
+      <c r="C60" s="27">
+        <v>150</v>
+      </c>
+      <c r="D60" s="24">
         <v>6865</v>
       </c>
     </row>
@@ -2295,16 +1500,16 @@
       <c r="B61" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C61" s="21"/>
-      <c r="D61" s="22"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="24"/>
     </row>
     <row r="62" spans="1:4" ht="30.6">
       <c r="A62" s="20"/>
       <c r="B62" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="21"/>
-      <c r="D62" s="22"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="24"/>
     </row>
     <row r="63" spans="1:4" ht="20.399999999999999">
       <c r="A63" s="17">
@@ -2313,7 +1518,7 @@
       <c r="B63" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C63" s="23">
+      <c r="C63" s="18">
         <v>150</v>
       </c>
       <c r="D63" s="19">
@@ -2325,7 +1530,7 @@
       <c r="B64" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C64" s="23"/>
+      <c r="C64" s="18"/>
       <c r="D64" s="19"/>
     </row>
     <row r="65" spans="1:4" ht="30.6">
@@ -2333,7 +1538,7 @@
       <c r="B65" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C65" s="23"/>
+      <c r="C65" s="18"/>
       <c r="D65" s="19"/>
     </row>
     <row r="66" spans="1:4" ht="20.399999999999999">
@@ -2343,10 +1548,10 @@
       <c r="B66" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C66" s="21">
-        <v>150</v>
-      </c>
-      <c r="D66" s="22">
+      <c r="C66" s="27">
+        <v>150</v>
+      </c>
+      <c r="D66" s="24">
         <v>6565</v>
       </c>
     </row>
@@ -2355,16 +1560,16 @@
       <c r="B67" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C67" s="21"/>
-      <c r="D67" s="22"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="24"/>
     </row>
     <row r="68" spans="1:4" ht="30.6">
       <c r="A68" s="20"/>
       <c r="B68" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C68" s="21"/>
-      <c r="D68" s="22"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="24"/>
     </row>
     <row r="69" spans="1:4" ht="20.399999999999999">
       <c r="A69" s="17">
@@ -2373,7 +1578,7 @@
       <c r="B69" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="23">
+      <c r="C69" s="18">
         <v>150</v>
       </c>
       <c r="D69" s="19">
@@ -2385,7 +1590,7 @@
       <c r="B70" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C70" s="23"/>
+      <c r="C70" s="18"/>
       <c r="D70" s="19"/>
     </row>
     <row r="71" spans="1:4" ht="30.6">
@@ -2393,7 +1598,7 @@
       <c r="B71" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C71" s="23"/>
+      <c r="C71" s="18"/>
       <c r="D71" s="19"/>
     </row>
     <row r="72" spans="1:4" ht="20.399999999999999">
@@ -2403,10 +1608,10 @@
       <c r="B72" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C72" s="21">
-        <v>150</v>
-      </c>
-      <c r="D72" s="22">
+      <c r="C72" s="27">
+        <v>150</v>
+      </c>
+      <c r="D72" s="24">
         <v>6265</v>
       </c>
     </row>
@@ -2415,16 +1620,16 @@
       <c r="B73" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C73" s="21"/>
-      <c r="D73" s="22"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="24"/>
     </row>
     <row r="74" spans="1:4" ht="30.6">
       <c r="A74" s="20"/>
       <c r="B74" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="21"/>
-      <c r="D74" s="22"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="24"/>
     </row>
     <row r="75" spans="1:4" ht="20.399999999999999">
       <c r="A75" s="17">
@@ -2433,7 +1638,7 @@
       <c r="B75" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C75" s="23">
+      <c r="C75" s="18">
         <v>150</v>
       </c>
       <c r="D75" s="19">
@@ -2445,7 +1650,7 @@
       <c r="B76" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="23"/>
+      <c r="C76" s="18"/>
       <c r="D76" s="19"/>
     </row>
     <row r="77" spans="1:4" ht="30.6">
@@ -2453,7 +1658,7 @@
       <c r="B77" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C77" s="23"/>
+      <c r="C77" s="18"/>
       <c r="D77" s="19"/>
     </row>
     <row r="78" spans="1:4" ht="20.399999999999999">
@@ -2463,10 +1668,10 @@
       <c r="B78" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C78" s="21">
+      <c r="C78" s="27">
         <v>300</v>
       </c>
-      <c r="D78" s="22">
+      <c r="D78" s="24">
         <v>5965</v>
       </c>
     </row>
@@ -2475,16 +1680,16 @@
       <c r="B79" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C79" s="21"/>
-      <c r="D79" s="22"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="24"/>
     </row>
     <row r="80" spans="1:4" ht="30.6">
       <c r="A80" s="20"/>
       <c r="B80" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C80" s="21"/>
-      <c r="D80" s="22"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="24"/>
     </row>
     <row r="81" spans="1:4" ht="20.399999999999999">
       <c r="A81" s="17">
@@ -2493,7 +1698,7 @@
       <c r="B81" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="23">
+      <c r="C81" s="18">
         <v>150</v>
       </c>
       <c r="D81" s="19">
@@ -2505,7 +1710,7 @@
       <c r="B82" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C82" s="23"/>
+      <c r="C82" s="18"/>
       <c r="D82" s="19"/>
     </row>
     <row r="83" spans="1:4" ht="20.399999999999999">
@@ -2513,7 +1718,7 @@
       <c r="B83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="23"/>
+      <c r="C83" s="18"/>
       <c r="D83" s="19"/>
     </row>
     <row r="84" spans="1:4" ht="20.399999999999999">
@@ -2523,10 +1728,10 @@
       <c r="B84" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C84" s="21">
-        <v>150</v>
-      </c>
-      <c r="D84" s="22">
+      <c r="C84" s="27">
+        <v>150</v>
+      </c>
+      <c r="D84" s="24">
         <v>5515</v>
       </c>
     </row>
@@ -2535,16 +1740,16 @@
       <c r="B85" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C85" s="21"/>
-      <c r="D85" s="22"/>
+      <c r="C85" s="27"/>
+      <c r="D85" s="24"/>
     </row>
     <row r="86" spans="1:4" ht="30.6">
       <c r="A86" s="20"/>
       <c r="B86" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C86" s="21"/>
-      <c r="D86" s="22"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="24"/>
     </row>
     <row r="87" spans="1:4" ht="20.399999999999999">
       <c r="A87" s="17">
@@ -2553,7 +1758,7 @@
       <c r="B87" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C87" s="23">
+      <c r="C87" s="18">
         <v>150</v>
       </c>
       <c r="D87" s="19">
@@ -2565,7 +1770,7 @@
       <c r="B88" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C88" s="23"/>
+      <c r="C88" s="18"/>
       <c r="D88" s="19"/>
     </row>
     <row r="89" spans="1:4" ht="30.6">
@@ -2573,7 +1778,7 @@
       <c r="B89" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C89" s="23"/>
+      <c r="C89" s="18"/>
       <c r="D89" s="19"/>
     </row>
     <row r="90" spans="1:4" ht="20.399999999999999">
@@ -2583,10 +1788,10 @@
       <c r="B90" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C90" s="21">
-        <v>150</v>
-      </c>
-      <c r="D90" s="22">
+      <c r="C90" s="27">
+        <v>150</v>
+      </c>
+      <c r="D90" s="24">
         <v>5215</v>
       </c>
     </row>
@@ -2595,16 +1800,16 @@
       <c r="B91" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C91" s="21"/>
-      <c r="D91" s="22"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="24"/>
     </row>
     <row r="92" spans="1:4" ht="20.399999999999999">
       <c r="A92" s="20"/>
       <c r="B92" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C92" s="21"/>
-      <c r="D92" s="22"/>
+      <c r="C92" s="27"/>
+      <c r="D92" s="24"/>
     </row>
     <row r="93" spans="1:4" ht="20.399999999999999">
       <c r="A93" s="17">
@@ -2613,7 +1818,7 @@
       <c r="B93" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C93" s="23">
+      <c r="C93" s="18">
         <v>150</v>
       </c>
       <c r="D93" s="19">
@@ -2625,7 +1830,7 @@
       <c r="B94" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C94" s="23"/>
+      <c r="C94" s="18"/>
       <c r="D94" s="19"/>
     </row>
     <row r="95" spans="1:4" ht="30.6">
@@ -2633,7 +1838,7 @@
       <c r="B95" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C95" s="23"/>
+      <c r="C95" s="18"/>
       <c r="D95" s="19"/>
     </row>
     <row r="96" spans="1:4" ht="20.399999999999999">
@@ -2643,10 +1848,10 @@
       <c r="B96" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C96" s="21">
-        <v>150</v>
-      </c>
-      <c r="D96" s="22">
+      <c r="C96" s="27">
+        <v>150</v>
+      </c>
+      <c r="D96" s="24">
         <v>4915</v>
       </c>
     </row>
@@ -2655,16 +1860,16 @@
       <c r="B97" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C97" s="21"/>
-      <c r="D97" s="22"/>
+      <c r="C97" s="27"/>
+      <c r="D97" s="24"/>
     </row>
     <row r="98" spans="1:4" ht="30.6">
       <c r="A98" s="20"/>
       <c r="B98" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C98" s="21"/>
-      <c r="D98" s="22"/>
+      <c r="C98" s="27"/>
+      <c r="D98" s="24"/>
     </row>
     <row r="99" spans="1:4" ht="20.399999999999999">
       <c r="A99" s="17">
@@ -2673,7 +1878,7 @@
       <c r="B99" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C99" s="23">
+      <c r="C99" s="18">
         <v>150</v>
       </c>
       <c r="D99" s="19">
@@ -2685,7 +1890,7 @@
       <c r="B100" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C100" s="23"/>
+      <c r="C100" s="18"/>
       <c r="D100" s="19"/>
     </row>
     <row r="101" spans="1:4" ht="30.6">
@@ -2693,7 +1898,7 @@
       <c r="B101" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C101" s="23"/>
+      <c r="C101" s="18"/>
       <c r="D101" s="19"/>
     </row>
     <row r="102" spans="1:4" ht="20.399999999999999">
@@ -2703,10 +1908,10 @@
       <c r="B102" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C102" s="21">
-        <v>150</v>
-      </c>
-      <c r="D102" s="22">
+      <c r="C102" s="27">
+        <v>150</v>
+      </c>
+      <c r="D102" s="24">
         <v>4615</v>
       </c>
     </row>
@@ -2715,16 +1920,16 @@
       <c r="B103" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C103" s="21"/>
-      <c r="D103" s="22"/>
+      <c r="C103" s="27"/>
+      <c r="D103" s="24"/>
     </row>
     <row r="104" spans="1:4" ht="20.399999999999999">
       <c r="A104" s="20"/>
       <c r="B104" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C104" s="21"/>
-      <c r="D104" s="22"/>
+      <c r="C104" s="27"/>
+      <c r="D104" s="24"/>
     </row>
     <row r="105" spans="1:4" ht="20.399999999999999">
       <c r="A105" s="17">
@@ -2733,7 +1938,7 @@
       <c r="B105" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C105" s="23">
+      <c r="C105" s="18">
         <v>300</v>
       </c>
       <c r="D105" s="19">
@@ -2745,7 +1950,7 @@
       <c r="B106" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C106" s="23"/>
+      <c r="C106" s="18"/>
       <c r="D106" s="19"/>
     </row>
     <row r="107" spans="1:4" ht="30.6">
@@ -2753,7 +1958,7 @@
       <c r="B107" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C107" s="23"/>
+      <c r="C107" s="18"/>
       <c r="D107" s="19"/>
     </row>
     <row r="108" spans="1:4" ht="20.399999999999999">
@@ -2763,10 +1968,10 @@
       <c r="B108" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C108" s="21">
-        <v>150</v>
-      </c>
-      <c r="D108" s="22">
+      <c r="C108" s="27">
+        <v>150</v>
+      </c>
+      <c r="D108" s="24">
         <v>4165</v>
       </c>
     </row>
@@ -2775,16 +1980,16 @@
       <c r="B109" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C109" s="21"/>
-      <c r="D109" s="22"/>
+      <c r="C109" s="27"/>
+      <c r="D109" s="24"/>
     </row>
     <row r="110" spans="1:4" ht="30.6">
       <c r="A110" s="20"/>
       <c r="B110" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C110" s="21"/>
-      <c r="D110" s="22"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="24"/>
     </row>
     <row r="111" spans="1:4" ht="20.399999999999999">
       <c r="A111" s="17">
@@ -2793,7 +1998,7 @@
       <c r="B111" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C111" s="23">
+      <c r="C111" s="18">
         <v>150</v>
       </c>
       <c r="D111" s="19">
@@ -2805,7 +2010,7 @@
       <c r="B112" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C112" s="23"/>
+      <c r="C112" s="18"/>
       <c r="D112" s="19"/>
     </row>
     <row r="113" spans="1:4" ht="30.6">
@@ -2813,7 +2018,7 @@
       <c r="B113" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C113" s="23"/>
+      <c r="C113" s="18"/>
       <c r="D113" s="19"/>
     </row>
     <row r="114" spans="1:4" ht="20.399999999999999">
@@ -2823,10 +2028,10 @@
       <c r="B114" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C114" s="21">
-        <v>150</v>
-      </c>
-      <c r="D114" s="22">
+      <c r="C114" s="27">
+        <v>150</v>
+      </c>
+      <c r="D114" s="24">
         <v>3865</v>
       </c>
     </row>
@@ -2835,16 +2040,16 @@
       <c r="B115" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C115" s="21"/>
-      <c r="D115" s="22"/>
+      <c r="C115" s="27"/>
+      <c r="D115" s="24"/>
     </row>
     <row r="116" spans="1:4" ht="30.6">
       <c r="A116" s="20"/>
       <c r="B116" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C116" s="21"/>
-      <c r="D116" s="22"/>
+      <c r="C116" s="27"/>
+      <c r="D116" s="24"/>
     </row>
     <row r="117" spans="1:4" ht="20.399999999999999">
       <c r="A117" s="17">
@@ -2853,7 +2058,7 @@
       <c r="B117" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C117" s="23">
+      <c r="C117" s="18">
         <v>150</v>
       </c>
       <c r="D117" s="19">
@@ -2865,7 +2070,7 @@
       <c r="B118" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C118" s="23"/>
+      <c r="C118" s="18"/>
       <c r="D118" s="19"/>
     </row>
     <row r="119" spans="1:4" ht="30.6">
@@ -2873,7 +2078,7 @@
       <c r="B119" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C119" s="23"/>
+      <c r="C119" s="18"/>
       <c r="D119" s="19"/>
     </row>
     <row r="120" spans="1:4" ht="20.399999999999999">
@@ -2883,10 +2088,10 @@
       <c r="B120" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C120" s="21">
+      <c r="C120" s="27">
         <v>300</v>
       </c>
-      <c r="D120" s="22">
+      <c r="D120" s="24">
         <v>3565</v>
       </c>
     </row>
@@ -2895,16 +2100,16 @@
       <c r="B121" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C121" s="21"/>
-      <c r="D121" s="22"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="24"/>
     </row>
     <row r="122" spans="1:4" ht="30.6">
       <c r="A122" s="20"/>
       <c r="B122" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C122" s="21"/>
-      <c r="D122" s="22"/>
+      <c r="C122" s="27"/>
+      <c r="D122" s="24"/>
     </row>
     <row r="123" spans="1:4" ht="20.399999999999999">
       <c r="A123" s="17">
@@ -2913,7 +2118,7 @@
       <c r="B123" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C123" s="23">
+      <c r="C123" s="18">
         <v>150</v>
       </c>
       <c r="D123" s="19">
@@ -2925,7 +2130,7 @@
       <c r="B124" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C124" s="23"/>
+      <c r="C124" s="18"/>
       <c r="D124" s="19"/>
     </row>
     <row r="125" spans="1:4" ht="20.399999999999999">
@@ -2933,7 +2138,7 @@
       <c r="B125" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C125" s="23"/>
+      <c r="C125" s="18"/>
       <c r="D125" s="19"/>
     </row>
     <row r="126" spans="1:4" ht="20.399999999999999">
@@ -2943,10 +2148,10 @@
       <c r="B126" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C126" s="21">
-        <v>150</v>
-      </c>
-      <c r="D126" s="22">
+      <c r="C126" s="27">
+        <v>150</v>
+      </c>
+      <c r="D126" s="24">
         <v>3115</v>
       </c>
     </row>
@@ -2955,16 +2160,16 @@
       <c r="B127" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C127" s="21"/>
-      <c r="D127" s="22"/>
+      <c r="C127" s="27"/>
+      <c r="D127" s="24"/>
     </row>
     <row r="128" spans="1:4" ht="30.6">
       <c r="A128" s="20"/>
       <c r="B128" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C128" s="21"/>
-      <c r="D128" s="22"/>
+      <c r="C128" s="27"/>
+      <c r="D128" s="24"/>
     </row>
     <row r="129" spans="1:4" ht="20.399999999999999">
       <c r="A129" s="17">
@@ -2973,7 +2178,7 @@
       <c r="B129" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C129" s="23">
+      <c r="C129" s="18">
         <v>150</v>
       </c>
       <c r="D129" s="19">
@@ -2985,7 +2190,7 @@
       <c r="B130" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C130" s="23"/>
+      <c r="C130" s="18"/>
       <c r="D130" s="19"/>
     </row>
     <row r="131" spans="1:4" ht="30.6">
@@ -2993,7 +2198,7 @@
       <c r="B131" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C131" s="23"/>
+      <c r="C131" s="18"/>
       <c r="D131" s="19"/>
     </row>
     <row r="132" spans="1:4" ht="20.399999999999999">
@@ -3003,10 +2208,10 @@
       <c r="B132" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C132" s="21">
-        <v>150</v>
-      </c>
-      <c r="D132" s="22">
+      <c r="C132" s="27">
+        <v>150</v>
+      </c>
+      <c r="D132" s="24">
         <v>2815</v>
       </c>
     </row>
@@ -3015,16 +2220,16 @@
       <c r="B133" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C133" s="21"/>
-      <c r="D133" s="22"/>
+      <c r="C133" s="27"/>
+      <c r="D133" s="24"/>
     </row>
     <row r="134" spans="1:4" ht="30.6">
       <c r="A134" s="20"/>
       <c r="B134" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C134" s="21"/>
-      <c r="D134" s="22"/>
+      <c r="C134" s="27"/>
+      <c r="D134" s="24"/>
     </row>
     <row r="135" spans="1:4" ht="20.399999999999999">
       <c r="A135" s="17">
@@ -3033,7 +2238,7 @@
       <c r="B135" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C135" s="23">
+      <c r="C135" s="18">
         <v>150</v>
       </c>
       <c r="D135" s="19">
@@ -3045,7 +2250,7 @@
       <c r="B136" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C136" s="23"/>
+      <c r="C136" s="18"/>
       <c r="D136" s="19"/>
     </row>
     <row r="137" spans="1:4" ht="20.399999999999999">
@@ -3053,7 +2258,7 @@
       <c r="B137" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C137" s="23"/>
+      <c r="C137" s="18"/>
       <c r="D137" s="19"/>
     </row>
     <row r="138" spans="1:4" ht="20.399999999999999">
@@ -3063,10 +2268,10 @@
       <c r="B138" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C138" s="21">
-        <v>150</v>
-      </c>
-      <c r="D138" s="22">
+      <c r="C138" s="27">
+        <v>150</v>
+      </c>
+      <c r="D138" s="24">
         <v>2515</v>
       </c>
     </row>
@@ -3075,16 +2280,16 @@
       <c r="B139" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C139" s="21"/>
-      <c r="D139" s="22"/>
+      <c r="C139" s="27"/>
+      <c r="D139" s="24"/>
     </row>
     <row r="140" spans="1:4" ht="30.6">
       <c r="A140" s="20"/>
       <c r="B140" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C140" s="21"/>
-      <c r="D140" s="22"/>
+      <c r="C140" s="27"/>
+      <c r="D140" s="24"/>
     </row>
     <row r="141" spans="1:4" ht="20.399999999999999">
       <c r="A141" s="17">
@@ -3093,7 +2298,7 @@
       <c r="B141" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C141" s="23">
+      <c r="C141" s="18">
         <v>600</v>
       </c>
       <c r="D141" s="19">
@@ -3105,7 +2310,7 @@
       <c r="B142" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C142" s="23"/>
+      <c r="C142" s="18"/>
       <c r="D142" s="19"/>
     </row>
     <row r="143" spans="1:4" ht="30.6">
@@ -3113,7 +2318,7 @@
       <c r="B143" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C143" s="23"/>
+      <c r="C143" s="18"/>
       <c r="D143" s="19"/>
     </row>
     <row r="144" spans="1:4" ht="20.399999999999999">
@@ -3123,10 +2328,10 @@
       <c r="B144" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C144" s="21">
-        <v>150</v>
-      </c>
-      <c r="D144" s="22">
+      <c r="C144" s="27">
+        <v>150</v>
+      </c>
+      <c r="D144" s="24">
         <v>1765</v>
       </c>
     </row>
@@ -3135,16 +2340,16 @@
       <c r="B145" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C145" s="21"/>
-      <c r="D145" s="22"/>
+      <c r="C145" s="27"/>
+      <c r="D145" s="24"/>
     </row>
     <row r="146" spans="1:4" ht="30.6">
       <c r="A146" s="20"/>
       <c r="B146" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C146" s="21"/>
-      <c r="D146" s="22"/>
+      <c r="C146" s="27"/>
+      <c r="D146" s="24"/>
     </row>
     <row r="147" spans="1:4" ht="20.399999999999999">
       <c r="A147" s="17">
@@ -3153,7 +2358,7 @@
       <c r="B147" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C147" s="23">
+      <c r="C147" s="18">
         <v>150</v>
       </c>
       <c r="D147" s="19">
@@ -3165,7 +2370,7 @@
       <c r="B148" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C148" s="23"/>
+      <c r="C148" s="18"/>
       <c r="D148" s="19"/>
     </row>
     <row r="149" spans="1:4" ht="30.6">
@@ -3173,7 +2378,7 @@
       <c r="B149" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C149" s="23"/>
+      <c r="C149" s="18"/>
       <c r="D149" s="19"/>
     </row>
     <row r="150" spans="1:4" ht="20.399999999999999">
@@ -3183,10 +2388,10 @@
       <c r="B150" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C150" s="21">
-        <v>150</v>
-      </c>
-      <c r="D150" s="22">
+      <c r="C150" s="27">
+        <v>150</v>
+      </c>
+      <c r="D150" s="24">
         <v>1465</v>
       </c>
     </row>
@@ -3195,16 +2400,16 @@
       <c r="B151" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C151" s="21"/>
-      <c r="D151" s="22"/>
+      <c r="C151" s="27"/>
+      <c r="D151" s="24"/>
     </row>
     <row r="152" spans="1:4" ht="30.6">
       <c r="A152" s="20"/>
       <c r="B152" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C152" s="21"/>
-      <c r="D152" s="22"/>
+      <c r="C152" s="27"/>
+      <c r="D152" s="24"/>
     </row>
     <row r="153" spans="1:4" ht="30.6">
       <c r="A153" s="17">
@@ -3213,7 +2418,7 @@
       <c r="B153" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C153" s="18">
+      <c r="C153" s="26">
         <v>-6.5</v>
       </c>
       <c r="D153" s="19">
@@ -3225,7 +2430,7 @@
       <c r="B154" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C154" s="18"/>
+      <c r="C154" s="26"/>
       <c r="D154" s="19"/>
     </row>
     <row r="155" spans="1:4" ht="20.399999999999999">
@@ -3235,10 +2440,10 @@
       <c r="B155" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C155" s="21">
-        <v>150</v>
-      </c>
-      <c r="D155" s="22">
+      <c r="C155" s="27">
+        <v>150</v>
+      </c>
+      <c r="D155" s="24">
         <v>1321.5</v>
       </c>
     </row>
@@ -3247,16 +2452,16 @@
       <c r="B156" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C156" s="21"/>
-      <c r="D156" s="22"/>
+      <c r="C156" s="27"/>
+      <c r="D156" s="24"/>
     </row>
     <row r="157" spans="1:4" ht="20.399999999999999">
       <c r="A157" s="20"/>
       <c r="B157" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C157" s="21"/>
-      <c r="D157" s="22"/>
+      <c r="C157" s="27"/>
+      <c r="D157" s="24"/>
     </row>
     <row r="158" spans="1:4" ht="20.399999999999999">
       <c r="A158" s="17">
@@ -3265,7 +2470,7 @@
       <c r="B158" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C158" s="23">
+      <c r="C158" s="18">
         <v>150</v>
       </c>
       <c r="D158" s="19">
@@ -3277,7 +2482,7 @@
       <c r="B159" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C159" s="23"/>
+      <c r="C159" s="18"/>
       <c r="D159" s="19"/>
     </row>
     <row r="160" spans="1:4" ht="30.6">
@@ -3285,7 +2490,7 @@
       <c r="B160" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C160" s="23"/>
+      <c r="C160" s="18"/>
       <c r="D160" s="19"/>
     </row>
     <row r="161" spans="1:4" ht="20.399999999999999">
@@ -3295,10 +2500,10 @@
       <c r="B161" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C161" s="21">
-        <v>150</v>
-      </c>
-      <c r="D161" s="22">
+      <c r="C161" s="27">
+        <v>150</v>
+      </c>
+      <c r="D161" s="24">
         <v>1021.5</v>
       </c>
     </row>
@@ -3307,16 +2512,16 @@
       <c r="B162" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C162" s="21"/>
-      <c r="D162" s="22"/>
+      <c r="C162" s="27"/>
+      <c r="D162" s="24"/>
     </row>
     <row r="163" spans="1:4" ht="30.6">
       <c r="A163" s="20"/>
       <c r="B163" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C163" s="21"/>
-      <c r="D163" s="22"/>
+      <c r="C163" s="27"/>
+      <c r="D163" s="24"/>
     </row>
     <row r="164" spans="1:4" ht="30.6">
       <c r="A164" s="17">
@@ -3325,7 +2530,7 @@
       <c r="B164" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C164" s="18">
+      <c r="C164" s="26">
         <v>-6.5</v>
       </c>
       <c r="D164" s="19">
@@ -3337,7 +2542,7 @@
       <c r="B165" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C165" s="18"/>
+      <c r="C165" s="26"/>
       <c r="D165" s="19"/>
     </row>
     <row r="166" spans="1:4" ht="30.6">
@@ -3347,10 +2552,10 @@
       <c r="B166" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C166" s="24">
+      <c r="C166" s="22">
         <v>-0.6</v>
       </c>
-      <c r="D166" s="22">
+      <c r="D166" s="24">
         <v>878</v>
       </c>
     </row>
@@ -3359,8 +2564,8 @@
       <c r="B167" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C167" s="24"/>
-      <c r="D167" s="22"/>
+      <c r="C167" s="22"/>
+      <c r="D167" s="24"/>
     </row>
     <row r="168" spans="1:4" ht="20.399999999999999">
       <c r="A168" s="17">
@@ -3369,7 +2574,7 @@
       <c r="B168" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C168" s="23">
+      <c r="C168" s="18">
         <v>300</v>
       </c>
       <c r="D168" s="19">
@@ -3381,7 +2586,7 @@
       <c r="B169" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C169" s="23"/>
+      <c r="C169" s="18"/>
       <c r="D169" s="19"/>
     </row>
     <row r="170" spans="1:4" ht="40.799999999999997">
@@ -3389,7 +2594,7 @@
       <c r="B170" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C170" s="23"/>
+      <c r="C170" s="18"/>
       <c r="D170" s="19"/>
     </row>
     <row r="171" spans="1:4" ht="20.399999999999999">
@@ -3399,10 +2604,10 @@
       <c r="B171" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C171" s="21">
-        <v>150</v>
-      </c>
-      <c r="D171" s="22">
+      <c r="C171" s="27">
+        <v>150</v>
+      </c>
+      <c r="D171" s="24">
         <v>578.6</v>
       </c>
     </row>
@@ -3411,16 +2616,16 @@
       <c r="B172" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C172" s="21"/>
-      <c r="D172" s="22"/>
+      <c r="C172" s="27"/>
+      <c r="D172" s="24"/>
     </row>
     <row r="173" spans="1:4" ht="30.6">
       <c r="A173" s="20"/>
       <c r="B173" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C173" s="21"/>
-      <c r="D173" s="22"/>
+      <c r="C173" s="27"/>
+      <c r="D173" s="24"/>
     </row>
     <row r="174" spans="1:4" ht="20.399999999999999">
       <c r="A174" s="17">
@@ -3429,7 +2634,7 @@
       <c r="B174" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C174" s="18">
+      <c r="C174" s="26">
         <v>-2050</v>
       </c>
       <c r="D174" s="19">
@@ -3441,7 +2646,7 @@
       <c r="B175" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C175" s="18"/>
+      <c r="C175" s="26"/>
       <c r="D175" s="19"/>
     </row>
     <row r="176" spans="1:4">
@@ -3449,7 +2654,7 @@
       <c r="B176" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C176" s="18"/>
+      <c r="C176" s="26"/>
       <c r="D176" s="19"/>
     </row>
     <row r="177" spans="1:4" ht="20.399999999999999">
@@ -3457,7 +2662,7 @@
       <c r="B177" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C177" s="18"/>
+      <c r="C177" s="26"/>
       <c r="D177" s="19"/>
     </row>
     <row r="178" spans="1:4" ht="20.399999999999999">
@@ -3467,10 +2672,10 @@
       <c r="B178" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C178" s="21">
-        <v>150</v>
-      </c>
-      <c r="D178" s="22">
+      <c r="C178" s="27">
+        <v>150</v>
+      </c>
+      <c r="D178" s="24">
         <v>2478.6</v>
       </c>
     </row>
@@ -3479,16 +2684,16 @@
       <c r="B179" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C179" s="21"/>
-      <c r="D179" s="22"/>
+      <c r="C179" s="27"/>
+      <c r="D179" s="24"/>
     </row>
     <row r="180" spans="1:4" ht="20.399999999999999">
       <c r="A180" s="20"/>
       <c r="B180" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C180" s="21"/>
-      <c r="D180" s="22"/>
+      <c r="C180" s="27"/>
+      <c r="D180" s="24"/>
     </row>
     <row r="181" spans="1:4" ht="20.399999999999999">
       <c r="A181" s="17">
@@ -3497,7 +2702,7 @@
       <c r="B181" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C181" s="23">
+      <c r="C181" s="18">
         <v>150</v>
       </c>
       <c r="D181" s="19">
@@ -3509,7 +2714,7 @@
       <c r="B182" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C182" s="23"/>
+      <c r="C182" s="18"/>
       <c r="D182" s="19"/>
     </row>
     <row r="183" spans="1:4" ht="30.6">
@@ -3517,7 +2722,7 @@
       <c r="B183" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C183" s="23"/>
+      <c r="C183" s="18"/>
       <c r="D183" s="19"/>
     </row>
     <row r="184" spans="1:4" ht="20.399999999999999">
@@ -3527,10 +2732,10 @@
       <c r="B184" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C184" s="21">
-        <v>150</v>
-      </c>
-      <c r="D184" s="22">
+      <c r="C184" s="27">
+        <v>150</v>
+      </c>
+      <c r="D184" s="24">
         <v>2178.6</v>
       </c>
     </row>
@@ -3539,16 +2744,16 @@
       <c r="B185" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C185" s="21"/>
-      <c r="D185" s="22"/>
+      <c r="C185" s="27"/>
+      <c r="D185" s="24"/>
     </row>
     <row r="186" spans="1:4" ht="30.6">
       <c r="A186" s="20"/>
       <c r="B186" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C186" s="21"/>
-      <c r="D186" s="22"/>
+      <c r="C186" s="27"/>
+      <c r="D186" s="24"/>
     </row>
     <row r="187" spans="1:4" ht="30.6">
       <c r="A187" s="17">
@@ -3557,7 +2762,7 @@
       <c r="B187" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C187" s="18">
+      <c r="C187" s="26">
         <v>-6.5</v>
       </c>
       <c r="D187" s="19">
@@ -3569,7 +2774,7 @@
       <c r="B188" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C188" s="18"/>
+      <c r="C188" s="26"/>
       <c r="D188" s="19"/>
     </row>
     <row r="189" spans="1:4" ht="20.399999999999999">
@@ -3579,10 +2784,10 @@
       <c r="B189" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C189" s="21">
-        <v>150</v>
-      </c>
-      <c r="D189" s="22">
+      <c r="C189" s="27">
+        <v>150</v>
+      </c>
+      <c r="D189" s="24">
         <v>2035.1</v>
       </c>
     </row>
@@ -3591,16 +2796,16 @@
       <c r="B190" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C190" s="21"/>
-      <c r="D190" s="22"/>
+      <c r="C190" s="27"/>
+      <c r="D190" s="24"/>
     </row>
     <row r="191" spans="1:4" ht="30.6">
       <c r="A191" s="20"/>
       <c r="B191" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C191" s="21"/>
-      <c r="D191" s="22"/>
+      <c r="C191" s="27"/>
+      <c r="D191" s="24"/>
     </row>
     <row r="192" spans="1:4" ht="20.399999999999999">
       <c r="A192" s="17">
@@ -3609,7 +2814,7 @@
       <c r="B192" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C192" s="23">
+      <c r="C192" s="18">
         <v>300</v>
       </c>
       <c r="D192" s="19">
@@ -3621,7 +2826,7 @@
       <c r="B193" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C193" s="23"/>
+      <c r="C193" s="18"/>
       <c r="D193" s="19"/>
     </row>
     <row r="194" spans="1:4" ht="30.6">
@@ -3629,7 +2834,7 @@
       <c r="B194" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C194" s="23"/>
+      <c r="C194" s="18"/>
       <c r="D194" s="19"/>
     </row>
     <row r="195" spans="1:4" ht="20.399999999999999">
@@ -3639,10 +2844,10 @@
       <c r="B195" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C195" s="21">
-        <v>150</v>
-      </c>
-      <c r="D195" s="22">
+      <c r="C195" s="27">
+        <v>150</v>
+      </c>
+      <c r="D195" s="24">
         <v>1585.1</v>
       </c>
     </row>
@@ -3651,16 +2856,16 @@
       <c r="B196" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C196" s="21"/>
-      <c r="D196" s="22"/>
+      <c r="C196" s="27"/>
+      <c r="D196" s="24"/>
     </row>
     <row r="197" spans="1:4" ht="20.399999999999999">
       <c r="A197" s="20"/>
       <c r="B197" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C197" s="21"/>
-      <c r="D197" s="22"/>
+      <c r="C197" s="27"/>
+      <c r="D197" s="24"/>
     </row>
     <row r="198" spans="1:4" ht="20.399999999999999">
       <c r="A198" s="17">
@@ -3669,7 +2874,7 @@
       <c r="B198" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C198" s="23">
+      <c r="C198" s="18">
         <v>150</v>
       </c>
       <c r="D198" s="19">
@@ -3681,7 +2886,7 @@
       <c r="B199" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C199" s="23"/>
+      <c r="C199" s="18"/>
       <c r="D199" s="19"/>
     </row>
     <row r="200" spans="1:4" ht="30.6">
@@ -3689,7 +2894,7 @@
       <c r="B200" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C200" s="23"/>
+      <c r="C200" s="18"/>
       <c r="D200" s="19"/>
     </row>
     <row r="201" spans="1:4" ht="20.399999999999999">
@@ -3699,10 +2904,10 @@
       <c r="B201" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C201" s="21">
+      <c r="C201" s="27">
         <v>300</v>
       </c>
-      <c r="D201" s="22">
+      <c r="D201" s="24">
         <v>1285.0999999999999</v>
       </c>
     </row>
@@ -3711,16 +2916,16 @@
       <c r="B202" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C202" s="21"/>
-      <c r="D202" s="22"/>
+      <c r="C202" s="27"/>
+      <c r="D202" s="24"/>
     </row>
     <row r="203" spans="1:4" ht="40.799999999999997">
       <c r="A203" s="20"/>
       <c r="B203" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C203" s="21"/>
-      <c r="D203" s="22"/>
+      <c r="C203" s="27"/>
+      <c r="D203" s="24"/>
     </row>
     <row r="204" spans="1:4" ht="20.399999999999999">
       <c r="A204" s="17">
@@ -3729,7 +2934,7 @@
       <c r="B204" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C204" s="23">
+      <c r="C204" s="18">
         <v>150</v>
       </c>
       <c r="D204" s="19">
@@ -3741,7 +2946,7 @@
       <c r="B205" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C205" s="23"/>
+      <c r="C205" s="18"/>
       <c r="D205" s="19"/>
     </row>
     <row r="206" spans="1:4" ht="30.6">
@@ -3749,7 +2954,7 @@
       <c r="B206" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C206" s="23"/>
+      <c r="C206" s="18"/>
       <c r="D206" s="19"/>
     </row>
     <row r="207" spans="1:4" ht="30.6">
@@ -3759,10 +2964,10 @@
       <c r="B207" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C207" s="24">
+      <c r="C207" s="22">
         <v>-6.5</v>
       </c>
-      <c r="D207" s="22">
+      <c r="D207" s="24">
         <v>835.1</v>
       </c>
     </row>
@@ -3771,8 +2976,8 @@
       <c r="B208" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C208" s="24"/>
-      <c r="D208" s="22"/>
+      <c r="C208" s="22"/>
+      <c r="D208" s="24"/>
     </row>
     <row r="209" spans="1:4" ht="30.6">
       <c r="A209" s="17">
@@ -3781,7 +2986,7 @@
       <c r="B209" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C209" s="18">
+      <c r="C209" s="26">
         <v>-2.1</v>
       </c>
       <c r="D209" s="19">
@@ -3793,7 +2998,7 @@
       <c r="B210" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C210" s="18"/>
+      <c r="C210" s="26"/>
       <c r="D210" s="19"/>
     </row>
     <row r="211" spans="1:4" ht="20.399999999999999">
@@ -3803,10 +3008,10 @@
       <c r="B211" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C211" s="21">
-        <v>150</v>
-      </c>
-      <c r="D211" s="22">
+      <c r="C211" s="27">
+        <v>150</v>
+      </c>
+      <c r="D211" s="24">
         <v>843.7</v>
       </c>
     </row>
@@ -3815,16 +3020,16 @@
       <c r="B212" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C212" s="21"/>
-      <c r="D212" s="22"/>
+      <c r="C212" s="27"/>
+      <c r="D212" s="24"/>
     </row>
     <row r="213" spans="1:4" ht="30.6">
       <c r="A213" s="20"/>
       <c r="B213" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C213" s="21"/>
-      <c r="D213" s="22"/>
+      <c r="C213" s="27"/>
+      <c r="D213" s="24"/>
     </row>
     <row r="214" spans="1:4" ht="20.399999999999999">
       <c r="A214" s="17">
@@ -3833,7 +3038,7 @@
       <c r="B214" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C214" s="23">
+      <c r="C214" s="18">
         <v>150</v>
       </c>
       <c r="D214" s="19">
@@ -3845,7 +3050,7 @@
       <c r="B215" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C215" s="23"/>
+      <c r="C215" s="18"/>
       <c r="D215" s="19"/>
     </row>
     <row r="216" spans="1:4" ht="20.399999999999999">
@@ -3853,7 +3058,7 @@
       <c r="B216" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C216" s="23"/>
+      <c r="C216" s="18"/>
       <c r="D216" s="19"/>
     </row>
     <row r="217" spans="1:4" ht="30.6" customHeight="1">
@@ -3863,10 +3068,10 @@
       <c r="B217" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C217" s="24">
+      <c r="C217" s="22">
         <v>-341.67</v>
       </c>
-      <c r="D217" s="22">
+      <c r="D217" s="24">
         <v>543.70000000000005</v>
       </c>
     </row>
@@ -3875,36 +3080,246 @@
       <c r="B218" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C218" s="24"/>
-      <c r="D218" s="22"/>
+      <c r="C218" s="22"/>
+      <c r="D218" s="24"/>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" s="20"/>
       <c r="B219" s="2">
         <v>10100086160634</v>
       </c>
-      <c r="C219" s="24"/>
-      <c r="D219" s="22"/>
+      <c r="C219" s="22"/>
+      <c r="D219" s="24"/>
     </row>
     <row r="220" spans="1:4" ht="30.6" customHeight="1">
       <c r="A220" s="20"/>
       <c r="B220" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C220" s="24"/>
-      <c r="D220" s="22"/>
+      <c r="C220" s="22"/>
+      <c r="D220" s="24"/>
     </row>
     <row r="221" spans="1:4" ht="31.2" thickBot="1">
-      <c r="A221" s="25"/>
+      <c r="A221" s="21"/>
       <c r="B221" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C221" s="26"/>
-      <c r="D221" s="27"/>
+      <c r="C221" s="23"/>
+      <c r="D221" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:C221" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="222">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="C63:C65"/>
+    <mergeCell ref="D63:D65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="D75:D77"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="D72:D74"/>
+    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="C87:C89"/>
+    <mergeCell ref="D87:D89"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="C90:C92"/>
+    <mergeCell ref="D90:D92"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="C84:C86"/>
+    <mergeCell ref="D84:D86"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="D99:D101"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="A93:A95"/>
+    <mergeCell ref="C93:C95"/>
+    <mergeCell ref="D93:D95"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="D96:D98"/>
+    <mergeCell ref="A111:A113"/>
+    <mergeCell ref="C111:C113"/>
+    <mergeCell ref="D111:D113"/>
+    <mergeCell ref="A114:A116"/>
+    <mergeCell ref="C114:C116"/>
+    <mergeCell ref="D114:D116"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="C105:C107"/>
+    <mergeCell ref="D105:D107"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="C108:C110"/>
+    <mergeCell ref="D108:D110"/>
+    <mergeCell ref="A123:A125"/>
+    <mergeCell ref="C123:C125"/>
+    <mergeCell ref="D123:D125"/>
+    <mergeCell ref="A126:A128"/>
+    <mergeCell ref="C126:C128"/>
+    <mergeCell ref="D126:D128"/>
+    <mergeCell ref="A117:A119"/>
+    <mergeCell ref="C117:C119"/>
+    <mergeCell ref="D117:D119"/>
+    <mergeCell ref="A120:A122"/>
+    <mergeCell ref="C120:C122"/>
+    <mergeCell ref="D120:D122"/>
+    <mergeCell ref="A135:A137"/>
+    <mergeCell ref="C135:C137"/>
+    <mergeCell ref="D135:D137"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="C138:C140"/>
+    <mergeCell ref="D138:D140"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="C129:C131"/>
+    <mergeCell ref="D129:D131"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="C132:C134"/>
+    <mergeCell ref="D132:D134"/>
+    <mergeCell ref="A147:A149"/>
+    <mergeCell ref="C147:C149"/>
+    <mergeCell ref="D147:D149"/>
+    <mergeCell ref="A150:A152"/>
+    <mergeCell ref="C150:C152"/>
+    <mergeCell ref="D150:D152"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="C141:C143"/>
+    <mergeCell ref="D141:D143"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="C144:C146"/>
+    <mergeCell ref="D144:D146"/>
+    <mergeCell ref="A158:A160"/>
+    <mergeCell ref="C158:C160"/>
+    <mergeCell ref="D158:D160"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="D161:D163"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="C155:C157"/>
+    <mergeCell ref="D155:D157"/>
+    <mergeCell ref="A168:A170"/>
+    <mergeCell ref="C168:C170"/>
+    <mergeCell ref="D168:D170"/>
+    <mergeCell ref="A171:A173"/>
+    <mergeCell ref="C171:C173"/>
+    <mergeCell ref="D171:D173"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="C164:C165"/>
+    <mergeCell ref="D164:D165"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="C166:C167"/>
+    <mergeCell ref="D166:D167"/>
+    <mergeCell ref="A181:A183"/>
+    <mergeCell ref="C181:C183"/>
+    <mergeCell ref="D181:D183"/>
+    <mergeCell ref="A184:A186"/>
+    <mergeCell ref="C184:C186"/>
+    <mergeCell ref="D184:D186"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="C174:C177"/>
+    <mergeCell ref="D174:D177"/>
+    <mergeCell ref="A178:A180"/>
+    <mergeCell ref="C178:C180"/>
+    <mergeCell ref="D178:D180"/>
+    <mergeCell ref="A192:A194"/>
+    <mergeCell ref="C192:C194"/>
+    <mergeCell ref="D192:D194"/>
+    <mergeCell ref="A195:A197"/>
+    <mergeCell ref="C195:C197"/>
+    <mergeCell ref="D195:D197"/>
+    <mergeCell ref="A187:A188"/>
+    <mergeCell ref="C187:C188"/>
+    <mergeCell ref="D187:D188"/>
+    <mergeCell ref="A189:A191"/>
+    <mergeCell ref="C189:C191"/>
+    <mergeCell ref="D189:D191"/>
+    <mergeCell ref="A204:A206"/>
+    <mergeCell ref="C204:C206"/>
+    <mergeCell ref="D204:D206"/>
+    <mergeCell ref="A207:A208"/>
+    <mergeCell ref="C207:C208"/>
+    <mergeCell ref="D207:D208"/>
+    <mergeCell ref="A198:A200"/>
+    <mergeCell ref="C198:C200"/>
+    <mergeCell ref="D198:D200"/>
+    <mergeCell ref="A201:A203"/>
+    <mergeCell ref="C201:C203"/>
+    <mergeCell ref="D201:D203"/>
     <mergeCell ref="A214:A216"/>
     <mergeCell ref="C214:C216"/>
     <mergeCell ref="D214:D216"/>
@@ -3917,216 +3332,6 @@
     <mergeCell ref="A211:A213"/>
     <mergeCell ref="C211:C213"/>
     <mergeCell ref="D211:D213"/>
-    <mergeCell ref="A204:A206"/>
-    <mergeCell ref="C204:C206"/>
-    <mergeCell ref="D204:D206"/>
-    <mergeCell ref="A207:A208"/>
-    <mergeCell ref="C207:C208"/>
-    <mergeCell ref="D207:D208"/>
-    <mergeCell ref="A198:A200"/>
-    <mergeCell ref="C198:C200"/>
-    <mergeCell ref="D198:D200"/>
-    <mergeCell ref="A201:A203"/>
-    <mergeCell ref="C201:C203"/>
-    <mergeCell ref="D201:D203"/>
-    <mergeCell ref="A192:A194"/>
-    <mergeCell ref="C192:C194"/>
-    <mergeCell ref="D192:D194"/>
-    <mergeCell ref="A195:A197"/>
-    <mergeCell ref="C195:C197"/>
-    <mergeCell ref="D195:D197"/>
-    <mergeCell ref="A187:A188"/>
-    <mergeCell ref="C187:C188"/>
-    <mergeCell ref="D187:D188"/>
-    <mergeCell ref="A189:A191"/>
-    <mergeCell ref="C189:C191"/>
-    <mergeCell ref="D189:D191"/>
-    <mergeCell ref="A181:A183"/>
-    <mergeCell ref="C181:C183"/>
-    <mergeCell ref="D181:D183"/>
-    <mergeCell ref="A184:A186"/>
-    <mergeCell ref="C184:C186"/>
-    <mergeCell ref="D184:D186"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="C174:C177"/>
-    <mergeCell ref="D174:D177"/>
-    <mergeCell ref="A178:A180"/>
-    <mergeCell ref="C178:C180"/>
-    <mergeCell ref="D178:D180"/>
-    <mergeCell ref="A168:A170"/>
-    <mergeCell ref="C168:C170"/>
-    <mergeCell ref="D168:D170"/>
-    <mergeCell ref="A171:A173"/>
-    <mergeCell ref="C171:C173"/>
-    <mergeCell ref="D171:D173"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="C164:C165"/>
-    <mergeCell ref="D164:D165"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="C166:C167"/>
-    <mergeCell ref="D166:D167"/>
-    <mergeCell ref="A158:A160"/>
-    <mergeCell ref="C158:C160"/>
-    <mergeCell ref="D158:D160"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="C161:C163"/>
-    <mergeCell ref="D161:D163"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="A155:A157"/>
-    <mergeCell ref="C155:C157"/>
-    <mergeCell ref="D155:D157"/>
-    <mergeCell ref="A147:A149"/>
-    <mergeCell ref="C147:C149"/>
-    <mergeCell ref="D147:D149"/>
-    <mergeCell ref="A150:A152"/>
-    <mergeCell ref="C150:C152"/>
-    <mergeCell ref="D150:D152"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="C141:C143"/>
-    <mergeCell ref="D141:D143"/>
-    <mergeCell ref="A144:A146"/>
-    <mergeCell ref="C144:C146"/>
-    <mergeCell ref="D144:D146"/>
-    <mergeCell ref="A135:A137"/>
-    <mergeCell ref="C135:C137"/>
-    <mergeCell ref="D135:D137"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="C138:C140"/>
-    <mergeCell ref="D138:D140"/>
-    <mergeCell ref="A129:A131"/>
-    <mergeCell ref="C129:C131"/>
-    <mergeCell ref="D129:D131"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="C132:C134"/>
-    <mergeCell ref="D132:D134"/>
-    <mergeCell ref="A123:A125"/>
-    <mergeCell ref="C123:C125"/>
-    <mergeCell ref="D123:D125"/>
-    <mergeCell ref="A126:A128"/>
-    <mergeCell ref="C126:C128"/>
-    <mergeCell ref="D126:D128"/>
-    <mergeCell ref="A117:A119"/>
-    <mergeCell ref="C117:C119"/>
-    <mergeCell ref="D117:D119"/>
-    <mergeCell ref="A120:A122"/>
-    <mergeCell ref="C120:C122"/>
-    <mergeCell ref="D120:D122"/>
-    <mergeCell ref="A111:A113"/>
-    <mergeCell ref="C111:C113"/>
-    <mergeCell ref="D111:D113"/>
-    <mergeCell ref="A114:A116"/>
-    <mergeCell ref="C114:C116"/>
-    <mergeCell ref="D114:D116"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="C105:C107"/>
-    <mergeCell ref="D105:D107"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="C108:C110"/>
-    <mergeCell ref="D108:D110"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="D99:D101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="A93:A95"/>
-    <mergeCell ref="C93:C95"/>
-    <mergeCell ref="D93:D95"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="C96:C98"/>
-    <mergeCell ref="D96:D98"/>
-    <mergeCell ref="A87:A89"/>
-    <mergeCell ref="C87:C89"/>
-    <mergeCell ref="D87:D89"/>
-    <mergeCell ref="A90:A92"/>
-    <mergeCell ref="C90:C92"/>
-    <mergeCell ref="D90:D92"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="D81:D83"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="C84:C86"/>
-    <mergeCell ref="D84:D86"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="D75:D77"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="D72:D74"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="C63:C65"/>
-    <mergeCell ref="D63:D65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4137,8 +3342,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5658,1224 +4863,4 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA793499-2F87-4161-B660-7261413A1647}">
-  <dimension ref="A1:E66"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="11">
-        <v>45112</v>
-      </c>
-      <c r="B2" s="12">
-        <v>150</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="8">
-        <v>45111</v>
-      </c>
-      <c r="B3" s="14">
-        <v>300</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="11">
-        <v>45108</v>
-      </c>
-      <c r="B4" s="12">
-        <v>150</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="8">
-        <v>45107</v>
-      </c>
-      <c r="B5" s="14">
-        <v>150</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="11">
-        <v>45083</v>
-      </c>
-      <c r="B6" s="12">
-        <v>150</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="8">
-        <v>45076</v>
-      </c>
-      <c r="B7" s="14">
-        <v>150</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="11">
-        <v>45047</v>
-      </c>
-      <c r="B8" s="12">
-        <v>300</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="8">
-        <v>45047</v>
-      </c>
-      <c r="B9" s="14">
-        <v>150</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="11">
-        <v>45047</v>
-      </c>
-      <c r="B10" s="12">
-        <v>150</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="8">
-        <v>45047</v>
-      </c>
-      <c r="B11" s="14">
-        <v>150</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="11">
-        <v>45047</v>
-      </c>
-      <c r="B12" s="12">
-        <v>150</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="8">
-        <v>45047</v>
-      </c>
-      <c r="B13" s="14">
-        <v>150</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="11">
-        <v>45044</v>
-      </c>
-      <c r="B14" s="12">
-        <v>150</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>120</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="8">
-        <v>45017</v>
-      </c>
-      <c r="B15" s="14">
-        <v>150</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="11">
-        <v>45016</v>
-      </c>
-      <c r="B16" s="12">
-        <v>150</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>122</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="8">
-        <v>45016</v>
-      </c>
-      <c r="B17" s="14">
-        <v>300</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>123</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="11">
-        <v>45015</v>
-      </c>
-      <c r="B18" s="12">
-        <v>150</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="8">
-        <v>44987</v>
-      </c>
-      <c r="B19" s="14">
-        <v>150</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="11">
-        <v>44987</v>
-      </c>
-      <c r="B20" s="12">
-        <v>150</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="8">
-        <v>44987</v>
-      </c>
-      <c r="B21" s="14">
-        <v>150</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="11">
-        <v>44986</v>
-      </c>
-      <c r="B22" s="12">
-        <v>150</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>128</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="8">
-        <v>44986</v>
-      </c>
-      <c r="B23" s="14">
-        <v>150</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>129</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="11">
-        <v>44981</v>
-      </c>
-      <c r="B24" s="12">
-        <v>150</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="8">
-        <v>44958</v>
-      </c>
-      <c r="B25" s="14">
-        <v>150</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="11">
-        <v>44958</v>
-      </c>
-      <c r="B26" s="12">
-        <v>300</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="8">
-        <v>44958</v>
-      </c>
-      <c r="B27" s="14">
-        <v>150</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
-        <v>133</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="11">
-        <v>44957</v>
-      </c>
-      <c r="B28" s="12">
-        <v>150</v>
-      </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>134</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="8">
-        <v>44928</v>
-      </c>
-      <c r="B29" s="14">
-        <v>150</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="11">
-        <v>44927</v>
-      </c>
-      <c r="B30" s="12">
-        <v>150</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="8">
-        <v>44926</v>
-      </c>
-      <c r="B31" s="14">
-        <v>150</v>
-      </c>
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>137</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="11">
-        <v>44922</v>
-      </c>
-      <c r="B32" s="12">
-        <v>150</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>138</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="8">
-        <v>44922</v>
-      </c>
-      <c r="B33" s="14">
-        <v>150</v>
-      </c>
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>139</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="11">
-        <v>44900</v>
-      </c>
-      <c r="B34" s="12">
-        <v>150</v>
-      </c>
-      <c r="C34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" t="s">
-        <v>140</v>
-      </c>
-      <c r="E34" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="8">
-        <v>44900</v>
-      </c>
-      <c r="B35" s="14">
-        <v>300</v>
-      </c>
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>141</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="11">
-        <v>44896</v>
-      </c>
-      <c r="B36" s="12">
-        <v>150</v>
-      </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>142</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="8">
-        <v>44896</v>
-      </c>
-      <c r="B37" s="14">
-        <v>150</v>
-      </c>
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="11">
-        <v>44879</v>
-      </c>
-      <c r="B38" s="12">
-        <v>150</v>
-      </c>
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="8">
-        <v>44866</v>
-      </c>
-      <c r="B39" s="14">
-        <v>150</v>
-      </c>
-      <c r="C39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" t="s">
-        <v>145</v>
-      </c>
-      <c r="E39" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="11">
-        <v>44866</v>
-      </c>
-      <c r="B40" s="12">
-        <v>300</v>
-      </c>
-      <c r="C40" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" t="s">
-        <v>146</v>
-      </c>
-      <c r="E40" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="8">
-        <v>44866</v>
-      </c>
-      <c r="B41" s="14">
-        <v>150</v>
-      </c>
-      <c r="C41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>147</v>
-      </c>
-      <c r="E41" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="11">
-        <v>44862</v>
-      </c>
-      <c r="B42" s="12">
-        <v>150</v>
-      </c>
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" t="s">
-        <v>148</v>
-      </c>
-      <c r="E42" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="8">
-        <v>44838</v>
-      </c>
-      <c r="B43" s="14">
-        <v>150</v>
-      </c>
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="s">
-        <v>149</v>
-      </c>
-      <c r="E43" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="11">
-        <v>44836</v>
-      </c>
-      <c r="B44" s="12">
-        <v>150</v>
-      </c>
-      <c r="C44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" t="s">
-        <v>150</v>
-      </c>
-      <c r="E44" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="8">
-        <v>44836</v>
-      </c>
-      <c r="B45" s="14">
-        <v>150</v>
-      </c>
-      <c r="C45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" t="s">
-        <v>151</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="11">
-        <v>44834</v>
-      </c>
-      <c r="B46" s="12">
-        <v>150</v>
-      </c>
-      <c r="C46" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="8">
-        <v>44833</v>
-      </c>
-      <c r="B47" s="14">
-        <v>600</v>
-      </c>
-      <c r="C47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>153</v>
-      </c>
-      <c r="E47" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="11">
-        <v>44813</v>
-      </c>
-      <c r="B48" s="12">
-        <v>150</v>
-      </c>
-      <c r="C48" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" t="s">
-        <v>154</v>
-      </c>
-      <c r="E48" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="8">
-        <v>44805</v>
-      </c>
-      <c r="B49" s="14">
-        <v>150</v>
-      </c>
-      <c r="C49" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" t="s">
-        <v>155</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="11">
-        <v>44805</v>
-      </c>
-      <c r="B50" s="12">
-        <v>150</v>
-      </c>
-      <c r="C50" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" t="s">
-        <v>156</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="11">
-        <v>44804</v>
-      </c>
-      <c r="B51" s="12">
-        <v>150</v>
-      </c>
-      <c r="C51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" t="s">
-        <v>157</v>
-      </c>
-      <c r="E51" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="8">
-        <v>44774</v>
-      </c>
-      <c r="B52" s="14">
-        <v>150</v>
-      </c>
-      <c r="C52" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" t="s">
-        <v>158</v>
-      </c>
-      <c r="E52" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="11">
-        <v>44774</v>
-      </c>
-      <c r="B53" s="12">
-        <v>150</v>
-      </c>
-      <c r="C53" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" t="s">
-        <v>159</v>
-      </c>
-      <c r="E53" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="8">
-        <v>44773</v>
-      </c>
-      <c r="B54" s="14">
-        <v>300</v>
-      </c>
-      <c r="C54" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" t="s">
-        <v>160</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="11">
-        <v>44772</v>
-      </c>
-      <c r="B55" s="12">
-        <v>150</v>
-      </c>
-      <c r="C55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" t="s">
-        <v>161</v>
-      </c>
-      <c r="E55" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="11">
-        <v>44771</v>
-      </c>
-      <c r="B56" s="12">
-        <v>150</v>
-      </c>
-      <c r="C56" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" t="s">
-        <v>162</v>
-      </c>
-      <c r="E56" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="8">
-        <v>44743</v>
-      </c>
-      <c r="B57" s="14">
-        <v>150</v>
-      </c>
-      <c r="C57" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" t="s">
-        <v>163</v>
-      </c>
-      <c r="E57" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="11">
-        <v>44743</v>
-      </c>
-      <c r="B58" s="12">
-        <v>150</v>
-      </c>
-      <c r="C58" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" t="s">
-        <v>164</v>
-      </c>
-      <c r="E58" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="11">
-        <v>44742</v>
-      </c>
-      <c r="B59" s="12">
-        <v>150</v>
-      </c>
-      <c r="C59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" t="s">
-        <v>165</v>
-      </c>
-      <c r="E59" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="8">
-        <v>44741</v>
-      </c>
-      <c r="B60" s="14">
-        <v>300</v>
-      </c>
-      <c r="C60" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" t="s">
-        <v>166</v>
-      </c>
-      <c r="E60" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="11">
-        <v>44741</v>
-      </c>
-      <c r="B61" s="12">
-        <v>150</v>
-      </c>
-      <c r="C61" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" t="s">
-        <v>167</v>
-      </c>
-      <c r="E61" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="8">
-        <v>44715</v>
-      </c>
-      <c r="B62" s="14">
-        <v>150</v>
-      </c>
-      <c r="C62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" t="s">
-        <v>168</v>
-      </c>
-      <c r="E62" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="11">
-        <v>44715</v>
-      </c>
-      <c r="B63" s="12">
-        <v>300</v>
-      </c>
-      <c r="C63" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" t="s">
-        <v>169</v>
-      </c>
-      <c r="E63" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="8">
-        <v>44714</v>
-      </c>
-      <c r="B64" s="14">
-        <v>150</v>
-      </c>
-      <c r="C64" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" t="s">
-        <v>170</v>
-      </c>
-      <c r="E64" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="11">
-        <v>44712</v>
-      </c>
-      <c r="B65" s="12">
-        <v>150</v>
-      </c>
-      <c r="C65" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" t="s">
-        <v>171</v>
-      </c>
-      <c r="E65" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="8">
-        <v>44708</v>
-      </c>
-      <c r="B66" s="14">
-        <v>150</v>
-      </c>
-      <c r="C66" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" t="s">
-        <v>172</v>
-      </c>
-      <c r="E66" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F580CDC-3659-4457-B801-C0F2976CA71C}">
-  <dimension ref="A3:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2">
-      <c r="A3" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="29">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" s="29">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="29">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="29">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="B8" s="29">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="29">
-        <v>11550</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>